<commit_message>
New run commands in NewFlukes2
Commands to run refstep program and produce data for a report.
</commit_message>
<xml_diff>
--- a/raw.2017.12.13.14.47.13.xlsx
+++ b/raw.2017.12.13.14.47.13.xlsx
@@ -9,6 +9,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -13038,4 +13040,654 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9999916158675644</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.090220841882094e-06</v>
+      </c>
+      <c r="D2" t="n">
+        <v>54.11722805817706</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.00000315248441</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.088869251436718e-06</v>
+      </c>
+      <c r="D3" t="n">
+        <v>47.65496536125958</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9999644893234579</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.097173042129777e-05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>51.10119936294383</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9999708503659723</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.023601576253771e-05</v>
+      </c>
+      <c r="D5" t="n">
+        <v>61.96396575355222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9999933900336889</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.009981742479961e-06</v>
+      </c>
+      <c r="D6" t="n">
+        <v>55.75913381049559</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-1.000031604198813</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.762232149208377e-06</v>
+      </c>
+      <c r="D7" t="n">
+        <v>41.93613821956109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9999832119785297</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.108533595146293e-06</v>
+      </c>
+      <c r="D8" t="n">
+        <v>53.6999714883345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>353</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.000049277892154</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.402893981848717e-06</v>
+      </c>
+      <c r="D9" t="n">
+        <v>60.52149569924817</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>350</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.999998640902493</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.610208643080906e-06</v>
+      </c>
+      <c r="D11" t="n">
+        <v>49.14124225983857</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9999977856214325</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.459234129138917e-06</v>
+      </c>
+      <c r="D12" t="n">
+        <v>31.14154209480693</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9999969221710352</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7.54742928375995e-06</v>
+      </c>
+      <c r="D13" t="n">
+        <v>34.32099055053742</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.000009799811334</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.727867001790709e-06</v>
+      </c>
+      <c r="D14" t="n">
+        <v>47.45334151602507</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.00000416183418</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.365936804738115e-06</v>
+      </c>
+      <c r="D15" t="n">
+        <v>51.08109566045659</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.000051071040077</v>
+      </c>
+      <c r="C16" t="n">
+        <v>7.472422039233697e-06</v>
+      </c>
+      <c r="D16" t="n">
+        <v>31.31480320137723</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.000001968219008</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5.6273997455357e-06</v>
+      </c>
+      <c r="D17" t="n">
+        <v>49.20401150932179</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-1.000046625637417</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5.825519414645741e-06</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45.30683409595279</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9999916158675644</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.090220841882094e-06</v>
+      </c>
+      <c r="D2" t="n">
+        <v>54.11722805817706</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.00000315248441</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.088869251436718e-06</v>
+      </c>
+      <c r="D3" t="n">
+        <v>47.65496536125958</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9999644893234579</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.097173042129777e-05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>51.10119936294383</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9999708503659723</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.023601576253771e-05</v>
+      </c>
+      <c r="D5" t="n">
+        <v>61.96396575355222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9999933900336889</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.009981742479961e-06</v>
+      </c>
+      <c r="D6" t="n">
+        <v>55.75913381049559</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-1.000031604198813</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.762232149208377e-06</v>
+      </c>
+      <c r="D7" t="n">
+        <v>41.93613821956109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9999832119785297</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.108533595146293e-06</v>
+      </c>
+      <c r="D8" t="n">
+        <v>53.6999714883345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>353</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.000049277892154</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.402893981848717e-06</v>
+      </c>
+      <c r="D9" t="n">
+        <v>60.52149569924817</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>350</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.999998640902493</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.610208643080906e-06</v>
+      </c>
+      <c r="D11" t="n">
+        <v>49.14124225983857</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9999977856214325</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.459234129138917e-06</v>
+      </c>
+      <c r="D12" t="n">
+        <v>31.14154209480693</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9999969221710352</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7.54742928375995e-06</v>
+      </c>
+      <c r="D13" t="n">
+        <v>34.32099055053742</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.000009799811334</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.727867001790709e-06</v>
+      </c>
+      <c r="D14" t="n">
+        <v>47.45334151602507</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.00000416183418</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.365936804738115e-06</v>
+      </c>
+      <c r="D15" t="n">
+        <v>51.08109566045659</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.000051071040077</v>
+      </c>
+      <c r="C16" t="n">
+        <v>7.472422039233697e-06</v>
+      </c>
+      <c r="D16" t="n">
+        <v>31.31480320137723</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.000001968219008</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5.6273997455357e-06</v>
+      </c>
+      <c r="D17" t="n">
+        <v>49.20401150932179</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-1.000046625637417</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5.825519414645741e-06</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45.30683409595279</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>